<commit_message>
Added a prototype dyr parse; Changed EXDC2 and TGOV1 parameters to follow PSS/E convention (all caps). Updated Kundur system correspondly.
</commit_message>
<xml_diff>
--- a/tests/kundur_full.xlsx
+++ b/tests/kundur_full.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/notebooks/kundur/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BABC913-F3E9-794C-8EDA-8EFA387CCB75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E127581F-5E67-6C47-9921-0F29AE3B4CF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10360" yWindow="1120" windowWidth="24240" windowHeight="19400" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1700" yWindow="460" windowWidth="31900" windowHeight="19340" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="119">
   <si>
     <t>idx</t>
   </si>
@@ -316,39 +316,6 @@
     <t>TGOV1_1</t>
   </si>
   <si>
-    <t>Tr</t>
-  </si>
-  <si>
-    <t>Ta</t>
-  </si>
-  <si>
-    <t>Tc</t>
-  </si>
-  <si>
-    <t>Tb</t>
-  </si>
-  <si>
-    <t>Te</t>
-  </si>
-  <si>
-    <t>Tf</t>
-  </si>
-  <si>
-    <t>Kf</t>
-  </si>
-  <si>
-    <t>Ka</t>
-  </si>
-  <si>
-    <t>Ke</t>
-  </si>
-  <si>
-    <t>vrmax</t>
-  </si>
-  <si>
-    <t>vrmin</t>
-  </si>
-  <si>
     <t>Ae</t>
   </si>
   <si>
@@ -368,13 +335,64 @@
   </si>
   <si>
     <t>Dt</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>TA</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>TE</t>
+  </si>
+  <si>
+    <t>KF1</t>
+  </si>
+  <si>
+    <t>TF1</t>
+  </si>
+  <si>
+    <t>KA</t>
+  </si>
+  <si>
+    <t>KE</t>
+  </si>
+  <si>
+    <t>VRMAX</t>
+  </si>
+  <si>
+    <t>VRMIN</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>SE1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>SE2</t>
+  </si>
+  <si>
+    <t>VMIN</t>
+  </si>
+  <si>
+    <t>VMAX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,6 +408,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -399,7 +424,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -422,15 +447,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1271,7 +1311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
@@ -3328,8 +3368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3354,10 +3394,10 @@
         <v>90</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>117</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
+        <v>118</v>
       </c>
       <c r="I1" t="s">
         <v>91</v>
@@ -3369,7 +3409,7 @@
         <v>93</v>
       </c>
       <c r="L1" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -3531,16 +3571,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N21" sqref="N21"/>
+      <selection pane="bottomLeft" activeCell="V2" sqref="V2:V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -3557,57 +3597,69 @@
         <v>88</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="S1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>97</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>108</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -3651,8 +3703,20 @@
       <c r="R2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2" s="3">
+        <v>0</v>
+      </c>
+      <c r="V2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3663,7 +3727,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -3707,8 +3771,20 @@
       <c r="R3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3" s="3">
+        <v>0</v>
+      </c>
+      <c r="V3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3719,7 +3795,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -3763,8 +3839,20 @@
       <c r="R4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4" s="3">
+        <v>0</v>
+      </c>
+      <c r="V4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3775,7 +3863,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -3817,6 +3905,18 @@
         <v>0</v>
       </c>
       <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5" s="3">
+        <v>0</v>
+      </c>
+      <c r="V5" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>